<commit_message>
Guion 10_08 para revisión de coordinacion
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion08/Escaleta_CN_10_08_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion08/Escaleta_CN_10_08_CO.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PLANETA 10 Y 11\CN_10_08_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion08\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -412,9 +412,6 @@
     <t>El equilibrio térmico</t>
   </si>
   <si>
-    <t>Interactivo que permite practicar con la temperatura, el calor y el equilibrio térmico</t>
-  </si>
-  <si>
     <t>Simulador F_Q</t>
   </si>
   <si>
@@ -445,9 +442,6 @@
     <t>Practica con las escalas de temperatura</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad que persigue aprender a convertir grados Celsius en Kelvin, grados Fahrenheit en Celsius y muchas otras combinaciones.  </t>
-  </si>
-  <si>
     <t>Consolidación</t>
   </si>
   <si>
@@ -559,12 +553,6 @@
     <t xml:space="preserve">Leyes de los gases ideales </t>
   </si>
   <si>
-    <t>Leyes de un gas ideal</t>
-  </si>
-  <si>
-    <t>Recurso que permite comprender el comportamiento a escala microscópica y macroscópica de un gas ideal</t>
-  </si>
-  <si>
     <t>Actividad para resolver problemas aplicando las leyes de los gases ideales</t>
   </si>
   <si>
@@ -574,9 +562,6 @@
     <t>Actividad que permite resolver problemas usando la ecuación de estado</t>
   </si>
   <si>
-    <t>Resuelve problemas con la ecuación de estado de un gas ideal</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ecuación de estado de un gas ideal </t>
   </si>
   <si>
@@ -664,12 +649,6 @@
     <t>Recurso M4A-01</t>
   </si>
   <si>
-    <t>Calor y temperatura</t>
-  </si>
-  <si>
-    <t>Interactivo que explica los temas de calor y temperatura y establece sus diferencias</t>
-  </si>
-  <si>
     <t>Diferencia calor y temperatura</t>
   </si>
   <si>
@@ -685,9 +664,6 @@
     <t>Las propiedades térmicas de la materia</t>
   </si>
   <si>
-    <t>Interactivo que permite conocer las propiedades termicas de la materia</t>
-  </si>
-  <si>
     <t>Hablasr sobre calor específico, capacidad calorífica, calor latente</t>
   </si>
   <si>
@@ -701,6 +677,30 @@
   </si>
   <si>
     <t>Competencias: observación del cambio de estado del agua</t>
+  </si>
+  <si>
+    <t>Interactivo que permite observar efectos relacionados con la temperatura, el calor y el equilibrio térmico</t>
+  </si>
+  <si>
+    <t>Interactivo que explica cuáles con las distintas unidades de medida de temperatura y su equivalencia</t>
+  </si>
+  <si>
+    <t>Actividad para practicar la conversión de grados Celsius en Kelvin, grados Fahrenheit en Celsius y muchas otras combinaciones</t>
+  </si>
+  <si>
+    <t>Interactivo que permite conocer las propiedades térmicas de la materia</t>
+  </si>
+  <si>
+    <t>Las leyes de un gas ideal</t>
+  </si>
+  <si>
+    <t>Interactivo que permite comprender el comportamiento a escala microscópica y macroscópica de un gas ideal</t>
+  </si>
+  <si>
+    <t>Resuelve problemas de gas ideal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resuelve problemas con la ecuación de estado de un gas ideal </t>
   </si>
 </sst>
 </file>
@@ -1508,12 +1508,60 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="44" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1531,54 +1579,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="44" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1729,6 +1729,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1764,6 +1781,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1942,9 +1976,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q24" sqref="Q24:U24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,7 +1992,7 @@
     <col min="7" max="7" width="87.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" style="35" customWidth="1"/>
     <col min="9" max="9" width="11" style="35" customWidth="1"/>
-    <col min="10" max="10" width="141.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74.140625" style="18" customWidth="1"/>
     <col min="11" max="11" width="13.140625" style="18" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" style="18" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" style="18" customWidth="1"/>
@@ -1973,94 +2007,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="74" t="s">
+      <c r="J1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="70" t="s">
+      <c r="L1" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="76" t="s">
+      <c r="M1" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="76"/>
-      <c r="O1" s="56" t="s">
+      <c r="N1" s="71"/>
+      <c r="O1" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="56" t="s">
+      <c r="P1" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="58" t="s">
+      <c r="Q1" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="58" t="s">
+      <c r="S1" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="60" t="s">
+      <c r="T1" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="58" t="s">
+      <c r="U1" s="74" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="71"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="66"/>
       <c r="M2" s="4" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="59"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="75"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -2084,10 +2118,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>126</v>
+        <v>215</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>19</v>
@@ -2098,7 +2132,7 @@
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
       <c r="O3" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P3" s="14" t="s">
         <v>19</v>
@@ -2107,16 +2141,16 @@
         <v>10</v>
       </c>
       <c r="R3" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="S3" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="T3" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="T3" s="17" t="s">
-        <v>131</v>
-      </c>
       <c r="U3" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2135,7 +2169,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="20"/>
       <c r="G4" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H4" s="8">
         <v>2</v>
@@ -2144,7 +2178,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K4" s="22" t="s">
         <v>19</v>
@@ -2164,16 +2198,16 @@
         <v>10</v>
       </c>
       <c r="R4" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="S4" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="S4" s="25" t="s">
-        <v>130</v>
-      </c>
       <c r="T4" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U4" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2190,11 +2224,11 @@
         <v>124</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="55" t="s">
-        <v>210</v>
+        <v>134</v>
       </c>
       <c r="H5" s="8">
         <v>3</v>
@@ -2203,7 +2237,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="K5" s="22" t="s">
         <v>19</v>
@@ -2216,7 +2250,7 @@
       </c>
       <c r="N5" s="24"/>
       <c r="O5" s="20" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="P5" s="20" t="s">
         <v>19</v>
@@ -2225,16 +2259,16 @@
         <v>10</v>
       </c>
       <c r="R5" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="S5" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="S5" s="25" t="s">
-        <v>130</v>
-      </c>
       <c r="T5" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="U5" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2251,11 +2285,11 @@
         <v>124</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H6" s="8">
         <v>4</v>
@@ -2264,7 +2298,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="K6" s="22" t="s">
         <v>19</v>
@@ -2284,16 +2318,16 @@
         <v>10</v>
       </c>
       <c r="R6" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="S6" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="S6" s="25" t="s">
-        <v>130</v>
-      </c>
       <c r="T6" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U6" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2310,11 +2344,11 @@
         <v>124</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="H7" s="8">
         <v>5</v>
@@ -2323,7 +2357,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K7" s="22" t="s">
         <v>20</v>
@@ -2343,16 +2377,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="S7" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="T7" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="S7" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="T7" s="27" t="s">
-        <v>142</v>
-      </c>
       <c r="U7" s="25" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="52" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2369,11 +2403,11 @@
         <v>124</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F8" s="42"/>
       <c r="G8" s="43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H8" s="8">
         <v>6</v>
@@ -2382,7 +2416,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K8" s="46" t="s">
         <v>20</v>
@@ -2402,16 +2436,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S8" s="49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T8" s="51" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="U8" s="49" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2425,14 +2459,14 @@
         <v>123</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="37" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H9" s="8">
         <v>7</v>
@@ -2441,7 +2475,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>20</v>
@@ -2454,7 +2488,7 @@
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="14" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="P9" s="14" t="s">
         <v>19</v>
@@ -2463,16 +2497,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="S9" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="T9" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="S9" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="T9" s="17" t="s">
-        <v>147</v>
-      </c>
       <c r="U9" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2486,14 +2520,14 @@
         <v>123</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H10" s="8">
         <v>8</v>
@@ -2502,7 +2536,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K10" s="22" t="s">
         <v>19</v>
@@ -2522,16 +2556,16 @@
         <v>10</v>
       </c>
       <c r="R10" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="S10" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="S10" s="25" t="s">
-        <v>130</v>
-      </c>
       <c r="T10" s="27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="U10" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2545,14 +2579,14 @@
         <v>123</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H11" s="8">
         <v>9</v>
@@ -2561,7 +2595,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K11" s="22" t="s">
         <v>19</v>
@@ -2581,16 +2615,16 @@
         <v>10</v>
       </c>
       <c r="R11" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="S11" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="S11" s="25" t="s">
-        <v>130</v>
-      </c>
       <c r="T11" s="27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="U11" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2604,14 +2638,14 @@
         <v>123</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H12" s="8">
         <v>10</v>
@@ -2620,7 +2654,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K12" s="22" t="s">
         <v>20</v>
@@ -2640,16 +2674,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="S12" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="T12" s="27" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="U12" s="25" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2663,14 +2697,14 @@
         <v>123</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H13" s="8">
         <v>11</v>
@@ -2679,7 +2713,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K13" s="22" t="s">
         <v>19</v>
@@ -2699,16 +2733,16 @@
         <v>8</v>
       </c>
       <c r="R13" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="S13" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="T13" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="S13" s="25" t="s">
+      <c r="U13" s="25" t="s">
         <v>159</v>
-      </c>
-      <c r="T13" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="U13" s="25" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2722,14 +2756,14 @@
         <v>123</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H14" s="8">
         <v>12</v>
@@ -2738,7 +2772,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>19</v>
@@ -2758,16 +2792,16 @@
         <v>10</v>
       </c>
       <c r="R14" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="S14" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="S14" s="25" t="s">
-        <v>130</v>
-      </c>
       <c r="T14" s="27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U14" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2781,23 +2815,23 @@
         <v>123</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H15" s="8">
         <v>13</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>20</v>
@@ -2811,22 +2845,22 @@
       </c>
       <c r="O15" s="20"/>
       <c r="P15" s="20" t="s">
-        <v>19</v>
+        <v>201</v>
       </c>
       <c r="Q15" s="25">
         <v>6</v>
       </c>
       <c r="R15" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S15" s="25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T15" s="27" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="U15" s="25" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="52" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2840,14 +2874,14 @@
         <v>123</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="43" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H16" s="8">
         <v>14</v>
@@ -2856,7 +2890,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="45" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K16" s="46" t="s">
         <v>20</v>
@@ -2876,16 +2910,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S16" s="49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T16" s="51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="U16" s="49" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2899,14 +2933,14 @@
         <v>123</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="37" t="s">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="H17" s="8">
         <v>15</v>
@@ -2915,7 +2949,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>176</v>
+        <v>220</v>
       </c>
       <c r="K17" s="11" t="s">
         <v>20</v>
@@ -2931,20 +2965,20 @@
       <c r="P17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="79">
+      <c r="Q17" s="56">
         <v>8</v>
       </c>
-      <c r="R17" s="79" t="s">
-        <v>129</v>
-      </c>
-      <c r="S17" s="79" t="s">
-        <v>220</v>
-      </c>
-      <c r="T17" s="79" t="s">
-        <v>221</v>
-      </c>
-      <c r="U17" s="79" t="s">
-        <v>219</v>
+      <c r="R17" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="S17" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="T17" s="56" t="s">
+        <v>213</v>
+      </c>
+      <c r="U17" s="56" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2958,14 +2992,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="9" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="H18" s="8">
         <v>16</v>
@@ -2974,7 +3008,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K18" s="22" t="s">
         <v>20</v>
@@ -2994,16 +3028,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S18" s="25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T18" s="27" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="U18" s="25" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3017,16 +3051,16 @@
         <v>123</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>180</v>
+        <v>222</v>
       </c>
       <c r="H19" s="8">
         <v>17</v>
@@ -3035,7 +3069,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K19" s="22" t="s">
         <v>20</v>
@@ -3049,22 +3083,22 @@
       </c>
       <c r="O19" s="20"/>
       <c r="P19" s="20" t="s">
-        <v>19</v>
+        <v>201</v>
       </c>
       <c r="Q19" s="25">
         <v>6</v>
       </c>
       <c r="R19" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S19" s="25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T19" s="27" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="U19" s="25" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:21" s="52" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3078,14 +3112,14 @@
         <v>123</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F20" s="42"/>
       <c r="G20" s="43" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="H20" s="8">
         <v>18</v>
@@ -3094,7 +3128,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="45" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="K20" s="46" t="s">
         <v>20</v>
@@ -3114,16 +3148,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S20" s="49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T20" s="51" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="U20" s="49" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -3137,14 +3171,14 @@
         <v>123</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="37" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H21" s="8">
         <v>19</v>
@@ -3153,7 +3187,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="K21" s="11" t="s">
         <v>20</v>
@@ -3173,16 +3207,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="T21" s="17" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="U21" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3196,14 +3230,14 @@
         <v>123</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="9" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="H22" s="8">
         <v>20</v>
@@ -3212,7 +3246,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K22" s="22" t="s">
         <v>20</v>
@@ -3232,16 +3266,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S22" s="25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T22" s="27" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="U22" s="25" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="52" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3255,14 +3289,14 @@
         <v>123</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F23" s="42"/>
       <c r="G23" s="43" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H23" s="8">
         <v>21</v>
@@ -3271,7 +3305,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="45" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K23" s="46" t="s">
         <v>20</v>
@@ -3291,16 +3325,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S23" s="49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T23" s="51" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="U23" s="49" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3314,12 +3348,12 @@
         <v>123</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E24" s="53"/>
       <c r="F24" s="54"/>
       <c r="G24" s="37" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H24" s="8">
         <v>22</v>
@@ -3328,7 +3362,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K24" s="11" t="s">
         <v>20</v>
@@ -3344,20 +3378,20 @@
       <c r="P24" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="79">
+      <c r="Q24" s="56">
         <v>8</v>
       </c>
-      <c r="R24" s="79" t="s">
-        <v>158</v>
-      </c>
-      <c r="S24" s="79" t="s">
+      <c r="R24" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="S24" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="T24" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="U24" s="56" t="s">
         <v>159</v>
-      </c>
-      <c r="T24" s="79" t="s">
-        <v>222</v>
-      </c>
-      <c r="U24" s="79" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -3371,7 +3405,7 @@
         <v>123</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="30"/>
@@ -3385,7 +3419,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K25" s="22" t="s">
         <v>20</v>
@@ -3414,12 +3448,12 @@
         <v>123</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="30"/>
       <c r="G26" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H26" s="8">
         <v>24</v>
@@ -3428,7 +3462,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="K26" s="22" t="s">
         <v>20</v>
@@ -3448,16 +3482,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S26" s="25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T26" s="27" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="U26" s="25" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3471,12 +3505,12 @@
         <v>123</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="20"/>
       <c r="G27" s="9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H27" s="8">
         <v>25</v>
@@ -3485,7 +3519,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="K27" s="22" t="s">
         <v>20</v>
@@ -3499,22 +3533,22 @@
       </c>
       <c r="O27" s="20"/>
       <c r="P27" s="20" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="Q27" s="25">
         <v>6</v>
       </c>
       <c r="R27" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S27" s="25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T27" s="27" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="U27" s="25" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4443,6 +4477,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4457,12 +4497,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>